<commit_message>
feat: add new template logic
</commit_message>
<xml_diff>
--- a/tests/data/template.xlsx
+++ b/tests/data/template.xlsx
@@ -1,37 +1,146 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\mos_chat-main\mos_chat-main\tests\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3680F4-765F-45C4-8E07-E6377676A5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test Cases" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+  <si>
+    <t>ชื่อ</t>
+  </si>
+  <si>
+    <t>นามสกุล</t>
+  </si>
+  <si>
+    <t>อายุ</t>
+  </si>
+  <si>
+    <t>หมายเหตุ</t>
+  </si>
+  <si>
+    <t>ผลการตรวจสอบ</t>
+  </si>
+  <si>
+    <t>ภาพผลการตรวจสอบ</t>
+  </si>
+  <si>
+    <t>Age below 18</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Age exactly 18</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Age above 18</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Edge case: zero age</t>
+  </si>
+  <si>
+    <t>Mos</t>
+  </si>
+  <si>
+    <t>Lnw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eiei </t>
+  </si>
+  <si>
+    <t>Krukri</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,81 +155,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,149 +470,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="61" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="72" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.8984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.69921875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="51.19921875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>ชื่อ</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>นามสกุล</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>อายุ</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>หมายเหตุ</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>ผลการตรวจสอบ</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>ภาพผลการตรวจสอบ</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Doe</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1">
         <v>17</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Age below 18</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Jane</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Smith</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
         <v>18</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Age exactly 18</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Johnson</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1">
         <v>25</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Age above 18</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Alice</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
         <v>15</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Age below 18</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Tom</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
         <v>0</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Edge case: zero age</t>
-        </is>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1">
+        <v>99</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add new template
</commit_message>
<xml_diff>
--- a/tests/data/template.xlsx
+++ b/tests/data/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\mos_chat-main\mos_chat-main\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3680F4-765F-45C4-8E07-E6377676A5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED27A7F-28DC-4FED-AAED-65DC85CB66E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>ชื่อ</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>ทดสอบระบบ</t>
+  </si>
+  <si>
+    <t>ภาษาไทยพิมพ์ได้ป่าว</t>
+  </si>
+  <si>
+    <t>Thai text</t>
   </si>
 </sst>
 </file>
@@ -471,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="61" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="72" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -592,6 +601,20 @@
         <v>22</v>
       </c>
     </row>
+    <row r="8" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>